<commit_message>
Both reuse and revision up can be displayed
</commit_message>
<xml_diff>
--- a/hot_plate.xlsx
+++ b/hot_plate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryozo/Dropbox/Client/ULVAC/ElectricDesignManagement/Tools/Revision-management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A4EBCE-FABE-744A-94DF-C3EC1588B9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811CF618-07AC-174F-80DA-CE1A7563CFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1940" windowWidth="16860" windowHeight="16720" xr2:uid="{E9733D3B-BDF0-5D43-BEDF-87B5B0FDBF9C}"/>
+    <workbookView xWindow="3180" yWindow="7340" windowWidth="16860" windowHeight="16720" xr2:uid="{E9733D3B-BDF0-5D43-BEDF-87B5B0FDBF9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Function</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>EE3273-614-03D</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -74,6 +70,10 @@
   </si>
   <si>
     <t>EE4383-614-03B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Drawing Type</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -482,7 +482,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -500,57 +500,57 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>